<commit_message>
Added logging to BlockTanksStats. Dashboards are now automatically posted to Discord. Now tracking clan DID
</commit_message>
<xml_diff>
--- a/Dashboards-test/DRONE.xlsx
+++ b/Dashboards-test/DRONE.xlsx
@@ -26,7 +26,7 @@
     <x:definedName name="DatesKDR">'KDR Per Day'!$D$1:$Q$1</x:definedName>
     <x:definedName name="DatesXP">'XP Per Day'!$E$1:$R$1</x:definedName>
     <x:definedName name="PlayersKDR">'KDR Per Day'!$A$2:$Q$51</x:definedName>
-    <x:definedName name="PlayersXP">'XP Per Day'!$A$2:$P$51</x:definedName>
+    <x:definedName name="PlayersXP">'XP Per Day'!$A$2:$R$51</x:definedName>
   </x:definedNames>
   <x:calcPr calcId="191029"/>
   <x:extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <x:si>
     <x:t>Player</x:t>
   </x:si>
@@ -232,7 +232,7 @@
     <x:t>- (/)</x:t>
   </x:si>
   <x:si>
-    <x:t>0,7 (538/732)</x:t>
+    <x:t>0,8 (741/922)</x:t>
   </x:si>
   <x:si>
     <x:t>0,0 (0/0)</x:t>
@@ -256,7 +256,10 @@
     <x:t>0,6 (156/256)</x:t>
   </x:si>
   <x:si>
-    <x:t>0,4 (17/41)</x:t>
+    <x:t>1,1 (203/190)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0,4 (21/53)</x:t>
   </x:si>
   <x:si>
     <x:t>1,5 (3/2)</x:t>
@@ -272,6 +275,9 @@
   </x:si>
   <x:si>
     <x:t>0,0 (0/14)</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0,3 (4/12)</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -780,16 +786,18 @@
       <x:c r="N2" s="16" t="s"/>
       <x:c r="O2" s="16" t="s"/>
       <x:c r="P2" s="16" t="s"/>
+      <x:c r="Q2" s="16" t="s"/>
+      <x:c r="R2" s="16" t="s"/>
     </x:row>
     <x:row r="3" spans="1:146" x14ac:dyDescent="0.25">
       <x:c r="B3" s="14" t="s">
         <x:v>4</x:v>
       </x:c>
       <x:c r="C3" s="15" t="n">
-        <x:v>1343.07734722217</x:v>
+        <x:v>1534.69911904756</x:v>
       </x:c>
       <x:c r="D3" s="15" t="n">
-        <x:v>581761.537437498</x:v>
+        <x:v>587130.396937498</x:v>
       </x:c>
       <x:c r="E3" s="16" t="n">
         <x:v>0</x:v>
@@ -826,6 +834,12 @@
       </x:c>
       <x:c r="P3" s="16" t="n">
         <x:v>4862.33020833309</x:v>
+      </x:c>
+      <x:c r="Q3" s="16" t="n">
+        <x:v>5368.85949999979</x:v>
+      </x:c>
+      <x:c r="R3" s="16" t="n">
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:146">
@@ -833,10 +847,10 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C4" s="15" t="n">
-        <x:v>38.2593958333357</x:v>
+        <x:v>41.6409464285742</x:v>
       </x:c>
       <x:c r="D4" s="15" t="n">
-        <x:v>157194.453875</x:v>
+        <x:v>157318.314375</x:v>
       </x:c>
       <x:c r="E4" s="16" t="n">
         <x:v>0</x:v>
@@ -873,6 +887,12 @@
       </x:c>
       <x:c r="P4" s="16" t="n">
         <x:v>90.9085000000196</x:v>
+      </x:c>
+      <x:c r="Q4" s="16" t="n">
+        <x:v>123.86050000001</x:v>
+      </x:c>
+      <x:c r="R4" s="16" t="n">
+        <x:v>0</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:146">
@@ -897,6 +917,8 @@
       <x:c r="N5" s="16" t="s"/>
       <x:c r="O5" s="16" t="s"/>
       <x:c r="P5" s="16" t="s"/>
+      <x:c r="Q5" s="16" t="s"/>
+      <x:c r="R5" s="16" t="s"/>
     </x:row>
     <x:row r="6" spans="1:146">
       <x:c r="B6" s="14" t="s">
@@ -920,6 +942,8 @@
       <x:c r="N6" s="16" t="s"/>
       <x:c r="O6" s="16" t="s"/>
       <x:c r="P6" s="16" t="s"/>
+      <x:c r="Q6" s="16" t="s"/>
+      <x:c r="R6" s="16" t="s"/>
     </x:row>
     <x:row r="7" spans="1:146">
       <x:c r="B7" s="14" t="s">
@@ -965,6 +989,12 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="P7" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="Q7" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R7" s="16" t="n">
         <x:v>0</x:v>
       </x:c>
     </x:row>
@@ -990,6 +1020,8 @@
       <x:c r="N8" s="16" t="s"/>
       <x:c r="O8" s="16" t="s"/>
       <x:c r="P8" s="16" t="s"/>
+      <x:c r="Q8" s="16" t="s"/>
+      <x:c r="R8" s="16" t="s"/>
     </x:row>
     <x:row r="9" spans="1:146">
       <x:c r="B9" s="14" t="s">
@@ -1013,6 +1045,8 @@
       <x:c r="N9" s="16" t="s"/>
       <x:c r="O9" s="16" t="s"/>
       <x:c r="P9" s="16" t="s"/>
+      <x:c r="Q9" s="16" t="s"/>
+      <x:c r="R9" s="16" t="s"/>
     </x:row>
     <x:row r="10" spans="1:146">
       <x:c r="B10" s="14" t="s">
@@ -1036,6 +1070,8 @@
       <x:c r="N10" s="16" t="s"/>
       <x:c r="O10" s="16" t="s"/>
       <x:c r="P10" s="16" t="s"/>
+      <x:c r="Q10" s="16" t="s"/>
+      <x:c r="R10" s="16" t="s"/>
     </x:row>
     <x:row r="11" spans="1:146">
       <x:c r="B11" s="14" t="s">
@@ -1059,6 +1095,8 @@
       <x:c r="N11" s="16" t="s"/>
       <x:c r="O11" s="16" t="s"/>
       <x:c r="P11" s="16" t="s"/>
+      <x:c r="Q11" s="16" t="s"/>
+      <x:c r="R11" s="16" t="s"/>
     </x:row>
     <x:row r="12" spans="1:146">
       <x:c r="B12" s="14" t="s">
@@ -1082,6 +1120,8 @@
       <x:c r="N12" s="16" t="s"/>
       <x:c r="O12" s="16" t="s"/>
       <x:c r="P12" s="16" t="s"/>
+      <x:c r="Q12" s="16" t="s"/>
+      <x:c r="R12" s="16" t="s"/>
     </x:row>
     <x:row r="13" spans="1:146" x14ac:dyDescent="0.25">
       <x:c r="B13" s="14" t="s">
@@ -1105,7 +1145,9 @@
       <x:c r="N13" s="16" t="s"/>
       <x:c r="O13" s="16" t="s"/>
       <x:c r="P13" s="16" t="s"/>
-      <x:c r="AC13" s="17" t="s"/>
+      <x:c r="Q13" s="16" t="s"/>
+      <x:c r="R13" s="16" t="s"/>
+      <x:c r="AE13" s="17" t="s"/>
     </x:row>
     <x:row r="14" spans="1:146" x14ac:dyDescent="0.25">
       <x:c r="B14" s="14" t="s">
@@ -1129,10 +1171,12 @@
       <x:c r="N14" s="16" t="s"/>
       <x:c r="O14" s="16" t="s"/>
       <x:c r="P14" s="16" t="s"/>
-      <x:c r="Z14" s="16" t="s"/>
-      <x:c r="AA14" s="16" t="s"/>
+      <x:c r="Q14" s="16" t="s"/>
+      <x:c r="R14" s="16" t="s"/>
       <x:c r="AB14" s="16" t="s"/>
       <x:c r="AC14" s="16" t="s"/>
+      <x:c r="AD14" s="16" t="s"/>
+      <x:c r="AE14" s="16" t="s"/>
     </x:row>
     <x:row r="15" spans="1:146">
       <x:c r="B15" s="14" t="s">
@@ -1156,6 +1200,8 @@
       <x:c r="N15" s="16" t="s"/>
       <x:c r="O15" s="16" t="s"/>
       <x:c r="P15" s="16" t="s"/>
+      <x:c r="Q15" s="16" t="s"/>
+      <x:c r="R15" s="16" t="s"/>
     </x:row>
     <x:row r="16" spans="1:146">
       <x:c r="B16" s="14" t="s">
@@ -1179,6 +1225,8 @@
       <x:c r="N16" s="16" t="s"/>
       <x:c r="O16" s="16" t="s"/>
       <x:c r="P16" s="16" t="s"/>
+      <x:c r="Q16" s="16" t="s"/>
+      <x:c r="R16" s="16" t="s"/>
     </x:row>
     <x:row r="17" spans="1:146">
       <x:c r="B17" s="14" t="s">
@@ -1224,6 +1272,12 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="P17" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="Q17" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R17" s="16" t="n">
         <x:v>0</x:v>
       </x:c>
     </x:row>
@@ -1249,6 +1303,8 @@
       <x:c r="N18" s="16" t="s"/>
       <x:c r="O18" s="16" t="s"/>
       <x:c r="P18" s="16" t="s"/>
+      <x:c r="Q18" s="16" t="s"/>
+      <x:c r="R18" s="16" t="s"/>
     </x:row>
     <x:row r="19" spans="1:146">
       <x:c r="B19" s="14" t="s">
@@ -1272,6 +1328,8 @@
       <x:c r="N19" s="16" t="s"/>
       <x:c r="O19" s="16" t="s"/>
       <x:c r="P19" s="16" t="s"/>
+      <x:c r="Q19" s="16" t="s"/>
+      <x:c r="R19" s="16" t="s"/>
     </x:row>
     <x:row r="20" spans="1:146">
       <x:c r="B20" s="14" t="s">
@@ -1295,6 +1353,8 @@
       <x:c r="N20" s="16" t="s"/>
       <x:c r="O20" s="16" t="s"/>
       <x:c r="P20" s="16" t="s"/>
+      <x:c r="Q20" s="16" t="s"/>
+      <x:c r="R20" s="16" t="s"/>
     </x:row>
     <x:row r="21" spans="1:146">
       <x:c r="B21" s="14" t="s">
@@ -1318,6 +1378,8 @@
       <x:c r="N21" s="16" t="s"/>
       <x:c r="O21" s="16" t="s"/>
       <x:c r="P21" s="16" t="s"/>
+      <x:c r="Q21" s="16" t="s"/>
+      <x:c r="R21" s="16" t="s"/>
     </x:row>
     <x:row r="22" spans="1:146">
       <x:c r="B22" s="14" t="s">
@@ -1341,6 +1403,8 @@
       <x:c r="N22" s="16" t="s"/>
       <x:c r="O22" s="16" t="s"/>
       <x:c r="P22" s="16" t="s"/>
+      <x:c r="Q22" s="16" t="s"/>
+      <x:c r="R22" s="16" t="s"/>
     </x:row>
     <x:row r="23" spans="1:146">
       <x:c r="B23" s="14" t="s">
@@ -1364,6 +1428,8 @@
       <x:c r="N23" s="16" t="s"/>
       <x:c r="O23" s="16" t="s"/>
       <x:c r="P23" s="16" t="s"/>
+      <x:c r="Q23" s="16" t="s"/>
+      <x:c r="R23" s="16" t="s"/>
     </x:row>
     <x:row r="24" spans="1:146">
       <x:c r="B24" s="14" t="s">
@@ -1387,6 +1453,8 @@
       <x:c r="N24" s="16" t="s"/>
       <x:c r="O24" s="16" t="s"/>
       <x:c r="P24" s="16" t="s"/>
+      <x:c r="Q24" s="16" t="s"/>
+      <x:c r="R24" s="16" t="s"/>
     </x:row>
     <x:row r="25" spans="1:146">
       <x:c r="B25" s="14" t="s">
@@ -1410,6 +1478,8 @@
       <x:c r="N25" s="16" t="s"/>
       <x:c r="O25" s="16" t="s"/>
       <x:c r="P25" s="16" t="s"/>
+      <x:c r="Q25" s="16" t="s"/>
+      <x:c r="R25" s="16" t="s"/>
     </x:row>
     <x:row r="26" spans="1:146">
       <x:c r="B26" s="14" t="s">
@@ -1433,6 +1503,8 @@
       <x:c r="N26" s="16" t="s"/>
       <x:c r="O26" s="16" t="s"/>
       <x:c r="P26" s="16" t="s"/>
+      <x:c r="Q26" s="16" t="s"/>
+      <x:c r="R26" s="16" t="s"/>
     </x:row>
     <x:row r="27" spans="1:146">
       <x:c r="B27" s="14" t="s">
@@ -1456,6 +1528,8 @@
       <x:c r="N27" s="16" t="s"/>
       <x:c r="O27" s="16" t="s"/>
       <x:c r="P27" s="16" t="s"/>
+      <x:c r="Q27" s="16" t="s"/>
+      <x:c r="R27" s="16" t="s"/>
     </x:row>
     <x:row r="28" spans="1:146">
       <x:c r="B28" s="14" t="s">
@@ -1479,6 +1553,8 @@
       <x:c r="N28" s="16" t="s"/>
       <x:c r="O28" s="16" t="s"/>
       <x:c r="P28" s="16" t="s"/>
+      <x:c r="Q28" s="16" t="s"/>
+      <x:c r="R28" s="16" t="s"/>
     </x:row>
     <x:row r="29" spans="1:146">
       <x:c r="B29" s="14" t="s">
@@ -1502,6 +1578,8 @@
       <x:c r="N29" s="16" t="s"/>
       <x:c r="O29" s="16" t="s"/>
       <x:c r="P29" s="16" t="s"/>
+      <x:c r="Q29" s="16" t="s"/>
+      <x:c r="R29" s="16" t="s"/>
     </x:row>
     <x:row r="30" spans="1:146">
       <x:c r="B30" s="14" t="s">
@@ -1525,6 +1603,8 @@
       <x:c r="N30" s="16" t="s"/>
       <x:c r="O30" s="16" t="s"/>
       <x:c r="P30" s="16" t="s"/>
+      <x:c r="Q30" s="16" t="s"/>
+      <x:c r="R30" s="16" t="s"/>
     </x:row>
     <x:row r="31" spans="1:146">
       <x:c r="B31" s="14" t="s">
@@ -1548,6 +1628,8 @@
       <x:c r="N31" s="16" t="s"/>
       <x:c r="O31" s="16" t="s"/>
       <x:c r="P31" s="16" t="s"/>
+      <x:c r="Q31" s="16" t="s"/>
+      <x:c r="R31" s="16" t="s"/>
     </x:row>
     <x:row r="32" spans="1:146">
       <x:c r="B32" s="14" t="s">
@@ -1593,6 +1675,12 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="P32" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="Q32" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R32" s="16" t="n">
         <x:v>0</x:v>
       </x:c>
     </x:row>
@@ -1618,6 +1706,8 @@
       <x:c r="N33" s="16" t="s"/>
       <x:c r="O33" s="16" t="s"/>
       <x:c r="P33" s="16" t="s"/>
+      <x:c r="Q33" s="16" t="s"/>
+      <x:c r="R33" s="16" t="s"/>
     </x:row>
     <x:row r="34" spans="1:146">
       <x:c r="B34" s="14" t="s">
@@ -1641,6 +1731,8 @@
       <x:c r="N34" s="16" t="s"/>
       <x:c r="O34" s="16" t="s"/>
       <x:c r="P34" s="16" t="s"/>
+      <x:c r="Q34" s="16" t="s"/>
+      <x:c r="R34" s="16" t="s"/>
     </x:row>
     <x:row r="35" spans="1:146">
       <x:c r="B35" s="14" t="s">
@@ -1664,6 +1756,8 @@
       <x:c r="N35" s="16" t="s"/>
       <x:c r="O35" s="16" t="s"/>
       <x:c r="P35" s="16" t="s"/>
+      <x:c r="Q35" s="16" t="s"/>
+      <x:c r="R35" s="16" t="s"/>
     </x:row>
     <x:row r="36" spans="1:146">
       <x:c r="B36" s="14" t="s">
@@ -1709,6 +1803,12 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="P36" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="Q36" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R36" s="16" t="n">
         <x:v>0</x:v>
       </x:c>
     </x:row>
@@ -1734,6 +1834,8 @@
       <x:c r="N37" s="16" t="s"/>
       <x:c r="O37" s="16" t="s"/>
       <x:c r="P37" s="16" t="s"/>
+      <x:c r="Q37" s="16" t="s"/>
+      <x:c r="R37" s="16" t="s"/>
     </x:row>
     <x:row r="38" spans="1:146">
       <x:c r="B38" s="14" t="s">
@@ -1781,6 +1883,12 @@
       <x:c r="P38" s="16" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="Q38" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R38" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
     <x:row r="39" spans="1:146">
       <x:c r="B39" s="14" t="s">
@@ -1828,6 +1936,12 @@
       <x:c r="P39" s="16" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="Q39" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R39" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
     <x:row r="40" spans="1:146">
       <x:c r="B40" s="14" t="s">
@@ -1875,6 +1989,12 @@
       <x:c r="P40" s="16" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="Q40" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R40" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
     <x:row r="41" spans="1:146">
       <x:c r="B41" s="14" t="s">
@@ -1922,6 +2042,12 @@
       <x:c r="P41" s="16" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="Q41" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R41" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
     <x:row r="42" spans="1:146">
       <x:c r="B42" s="14" t="s">
@@ -1967,6 +2093,12 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="P42" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="Q42" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R42" s="16" t="n">
         <x:v>0</x:v>
       </x:c>
     </x:row>
@@ -1992,6 +2124,8 @@
       <x:c r="N43" s="16" t="s"/>
       <x:c r="O43" s="16" t="s"/>
       <x:c r="P43" s="16" t="s"/>
+      <x:c r="Q43" s="16" t="s"/>
+      <x:c r="R43" s="16" t="s"/>
     </x:row>
     <x:row r="44" spans="1:146">
       <x:c r="B44" s="14" t="s">
@@ -2015,6 +2149,8 @@
       <x:c r="N44" s="16" t="s"/>
       <x:c r="O44" s="16" t="s"/>
       <x:c r="P44" s="16" t="s"/>
+      <x:c r="Q44" s="16" t="s"/>
+      <x:c r="R44" s="16" t="s"/>
     </x:row>
     <x:row r="45" spans="1:146">
       <x:c r="B45" s="14" t="s">
@@ -2038,6 +2174,8 @@
       <x:c r="N45" s="16" t="s"/>
       <x:c r="O45" s="16" t="s"/>
       <x:c r="P45" s="16" t="s"/>
+      <x:c r="Q45" s="16" t="s"/>
+      <x:c r="R45" s="16" t="s"/>
     </x:row>
     <x:row r="46" spans="1:146">
       <x:c r="B46" s="14" t="s">
@@ -2061,6 +2199,8 @@
       <x:c r="N46" s="16" t="s"/>
       <x:c r="O46" s="16" t="s"/>
       <x:c r="P46" s="16" t="s"/>
+      <x:c r="Q46" s="16" t="s"/>
+      <x:c r="R46" s="16" t="s"/>
     </x:row>
     <x:row r="47" spans="1:146">
       <x:c r="B47" s="14" t="s">
@@ -2084,6 +2224,8 @@
       <x:c r="N47" s="16" t="s"/>
       <x:c r="O47" s="16" t="s"/>
       <x:c r="P47" s="16" t="s"/>
+      <x:c r="Q47" s="16" t="s"/>
+      <x:c r="R47" s="16" t="s"/>
     </x:row>
     <x:row r="48" spans="1:146">
       <x:c r="B48" s="14" t="s">
@@ -2107,6 +2249,8 @@
       <x:c r="N48" s="16" t="s"/>
       <x:c r="O48" s="16" t="s"/>
       <x:c r="P48" s="16" t="s"/>
+      <x:c r="Q48" s="16" t="s"/>
+      <x:c r="R48" s="16" t="s"/>
     </x:row>
     <x:row r="49" spans="1:146">
       <x:c r="B49" s="14" t="s">
@@ -2154,6 +2298,12 @@
       <x:c r="P49" s="16" t="n">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="Q49" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R49" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
     </x:row>
     <x:row r="50" spans="1:146">
       <x:c r="B50" s="14" t="s">
@@ -2199,6 +2349,12 @@
         <x:v>0</x:v>
       </x:c>
       <x:c r="P50" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="Q50" s="16" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="R50" s="16" t="n">
         <x:v>0</x:v>
       </x:c>
     </x:row>
@@ -2233,8 +2389,8 @@
     <x:col min="11" max="12" width="13.270625" style="0" customWidth="1"/>
     <x:col min="13" max="13" width="14.700625" style="0" customWidth="1"/>
     <x:col min="14" max="14" width="13.270625" style="0" customWidth="1"/>
-    <x:col min="15" max="15" width="15.980625" style="0" customWidth="1"/>
-    <x:col min="16" max="17" width="13.270625" style="0" customWidth="1"/>
+    <x:col min="15" max="16" width="15.980625" style="0" customWidth="1"/>
+    <x:col min="17" max="17" width="13.270625" style="0" customWidth="1"/>
     <x:col min="18" max="23" width="8" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
@@ -2382,10 +2538,10 @@
         <x:v>68</x:v>
       </x:c>
       <x:c r="P3" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="Q3" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:36">
@@ -2393,7 +2549,7 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="C4" s="18" t="s">
-        <x:v>69</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D4" s="19" t="s">
         <x:v>62</x:v>
@@ -2411,31 +2567,31 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="I4" s="19" t="s">
-        <x:v>70</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="J4" s="19" t="s">
-        <x:v>71</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="K4" s="19" t="s">
         <x:v>62</x:v>
       </x:c>
       <x:c r="L4" s="19" t="s">
-        <x:v>72</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="M4" s="19" t="s">
         <x:v>62</x:v>
       </x:c>
       <x:c r="N4" s="19" t="s">
-        <x:v>73</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="O4" s="19" t="s">
-        <x:v>74</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="P4" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="Q4" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:36">
@@ -2582,10 +2738,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="P7" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Q7" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:36">
@@ -3082,10 +3238,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="P17" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Q17" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="18" spans="1:36">
@@ -3832,10 +3988,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="P32" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Q32" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="33" spans="1:36">
@@ -4032,10 +4188,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="P36" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Q36" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="37" spans="1:36">
@@ -4132,10 +4288,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="P38" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Q38" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="39" spans="1:36">
@@ -4182,10 +4338,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="P39" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Q39" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="40" spans="1:36">
@@ -4232,10 +4388,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="P40" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Q40" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="41" spans="1:36">
@@ -4282,10 +4438,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="P41" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Q41" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="42" spans="1:36">
@@ -4332,10 +4488,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="P42" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Q42" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="43" spans="1:36">
@@ -4682,10 +4838,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="P49" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Q49" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
     <x:row r="50" spans="1:36">
@@ -4732,10 +4888,10 @@
         <x:v>62</x:v>
       </x:c>
       <x:c r="P50" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="Q50" s="19" t="s">
-        <x:v>60</x:v>
+        <x:v>62</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>